<commit_message>
Falta formatar o relatorio
</commit_message>
<xml_diff>
--- a/Trabalho 4/trabalho 4.xlsx
+++ b/Trabalho 4/trabalho 4.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>Raio [m]</t>
   </si>
@@ -69,13 +69,28 @@
   </si>
   <si>
     <t>0,055</t>
+  </si>
+  <si>
+    <t>t [s]</t>
+  </si>
+  <si>
+    <t>Períodos</t>
+  </si>
+  <si>
+    <t>ε</t>
+  </si>
+  <si>
+    <t>0,914</t>
+  </si>
+  <si>
+    <t>3,06</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -88,6 +103,12 @@
       <color rgb="FF000000"/>
       <name val="Courier New"/>
       <family val="3"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -131,7 +152,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -144,6 +165,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="3" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -161,6 +188,60 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>695325</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>157162</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="65" cy="172227"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="TextBox 1"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5943600" y="2252662"/>
+          <a:ext cx="65" cy="172227"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -426,10 +507,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="D4:K16"/>
+  <dimension ref="D4:K24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="G29" sqref="G29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -437,7 +518,7 @@
     <col min="5" max="5" width="18.85546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="6.5703125" customWidth="1"/>
     <col min="7" max="8" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.140625" customWidth="1"/>
+    <col min="9" max="9" width="11.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="4" spans="4:11" x14ac:dyDescent="0.25">
@@ -634,8 +715,102 @@
         <v>-5.499999999999261E-2</v>
       </c>
     </row>
+    <row r="18" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D18" s="1"/>
+      <c r="E18" s="1"/>
+      <c r="F18" s="1"/>
+      <c r="G18" s="1"/>
+      <c r="H18" s="1"/>
+      <c r="I18" s="1"/>
+      <c r="J18" s="1"/>
+    </row>
+    <row r="19" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D19" s="1"/>
+      <c r="E19" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="F19" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G19" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="H19" s="1"/>
+      <c r="I19" s="1"/>
+      <c r="J19" s="1"/>
+    </row>
+    <row r="20" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D20" s="1"/>
+      <c r="E20" s="7">
+        <v>0.01</v>
+      </c>
+      <c r="F20" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="G20" s="4">
+        <v>22</v>
+      </c>
+      <c r="H20" s="1"/>
+      <c r="I20" s="1"/>
+      <c r="J20" s="1"/>
+    </row>
+    <row r="21" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D21" s="1"/>
+      <c r="E21" s="7">
+        <v>1E-3</v>
+      </c>
+      <c r="F21" s="5">
+        <v>1182</v>
+      </c>
+      <c r="G21" s="4">
+        <v>29</v>
+      </c>
+      <c r="H21" s="1"/>
+      <c r="I21" s="1"/>
+      <c r="J21" s="1"/>
+    </row>
+    <row r="22" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D22" s="1"/>
+      <c r="E22" s="7">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="F22" s="5">
+        <v>1718</v>
+      </c>
+      <c r="G22" s="4">
+        <v>42</v>
+      </c>
+      <c r="H22" s="1"/>
+      <c r="I22" s="1"/>
+      <c r="J22" s="1"/>
+    </row>
+    <row r="23" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D23" s="1"/>
+      <c r="E23" s="7">
+        <v>1E-10</v>
+      </c>
+      <c r="F23" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="G23" s="4">
+        <v>76</v>
+      </c>
+      <c r="H23" s="1"/>
+      <c r="I23" s="1"/>
+      <c r="J23" s="1"/>
+    </row>
+    <row r="24" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D24" s="1"/>
+      <c r="E24" s="1"/>
+      <c r="F24" s="1"/>
+      <c r="G24" s="1"/>
+      <c r="H24" s="1"/>
+      <c r="I24" s="1"/>
+      <c r="J24" s="1"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>